<commit_message>
features2 and nn_model2 updated
</commit_message>
<xml_diff>
--- a/output/features/feature_ideas_v2.xlsx
+++ b/output/features/feature_ideas_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward Sims\Documents\ml_projects\nerdycat\nfl-big-data-bowl\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward Sims\Documents\ml_projects\nerdycat\nfl-big-data-bowl\output\features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706F10DC-DB3C-47A3-81A1-186CF5E8F4B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DAA7C5-20CB-425D-9DF2-FCAD69CB9F29}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A745776-B911-4206-8911-3B0816B3A891}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="366">
   <si>
     <t>PlayId</t>
   </si>
@@ -1093,6 +1093,42 @@
   </si>
   <si>
     <t>A,S etc of general positions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WR fake or block? </t>
+  </si>
+  <si>
+    <t>use dir and otation of DB</t>
+  </si>
+  <si>
+    <t>Lead blocker features</t>
+  </si>
+  <si>
+    <t>how many offensive player blocking</t>
+  </si>
+  <si>
+    <t>winning blocks?</t>
+  </si>
+  <si>
+    <t>can we use weight, height, speed and dir to estimate if winning a block?</t>
+  </si>
+  <si>
+    <t>how far away are dbs?</t>
+  </si>
+  <si>
+    <t>how far did the wrs block/get them to bite?</t>
+  </si>
+  <si>
+    <t>IsBlitz</t>
+  </si>
+  <si>
+    <t>Look at edge rushers too</t>
+  </si>
+  <si>
+    <t>angles of blocking</t>
+  </si>
+  <si>
+    <t>watch out for illegal blocking - remove where necessary</t>
   </si>
 </sst>
 </file>
@@ -1595,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19A3A37-5DA0-43E0-B55F-7B9F3DDB721C}">
-  <dimension ref="A1:AA207"/>
+  <dimension ref="A1:AA214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A209" sqref="A209"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B214" sqref="B214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2032,708 +2068,698 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B56" s="12" t="s">
         <v>348</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B60" s="14" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="11" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="B60" s="12"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="13" t="s">
-        <v>311</v>
-      </c>
-      <c r="B61" s="14"/>
+      <c r="B61" s="12"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B62" s="14"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="B62" s="14"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="15" t="s">
+      <c r="B63" s="14"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="B63" s="16"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="B64" s="14"/>
+      <c r="B64" s="16"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B65" s="14"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B66" s="14"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="B67" s="14"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="B67" s="14"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="11" t="s">
+      <c r="B68" s="14"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="B68" s="12"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="B69" s="14"/>
+      <c r="B69" s="12"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="B70" s="14"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="B70" s="14"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="15" t="s">
+      <c r="B71" s="14"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="B71" s="16"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B72" s="14"/>
+      <c r="B72" s="16"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B73" s="14"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B74" s="14"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B75" s="14"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B75" s="14"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="11" t="s">
+      <c r="B76" s="14"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="B76" s="12"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="B77" s="14"/>
+      <c r="B77" s="12"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="B78" s="14"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="B78" s="14"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="15" t="s">
+      <c r="B79" s="14"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="B79" s="16"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="B80" s="14"/>
+      <c r="B80" s="16"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B81" s="14"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B82" s="14"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B83" s="14"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B83" s="14"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="11" t="s">
+      <c r="B84" s="14"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="B84" s="12"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="B85" s="14"/>
+      <c r="B85" s="12"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="B86" s="14"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="B86" s="14"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="15" t="s">
+      <c r="B87" s="14"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="15" t="s">
         <v>337</v>
       </c>
-      <c r="B87" s="16"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="B88" s="14"/>
+      <c r="B88" s="16"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B89" s="14"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B90" s="14"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B91" s="14"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B91" s="14"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="11" t="s">
+      <c r="B92" s="14"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B92" s="12" t="s">
+      <c r="B93" s="12" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="B93" s="14" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B96" s="14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="11" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B96" s="12" t="s">
+      <c r="B97" s="12" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="B97" s="14" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="B98" s="14" t="s">
+      <c r="B99" s="14" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="15" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B100" s="16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="11" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="B100" s="12" t="s">
+      <c r="B101" s="12" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="B101" s="14" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="B102" s="14" t="s">
+      <c r="B103" s="14" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="15" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="B103" s="16" t="s">
+      <c r="B104" s="16" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="11" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="B104" s="12" t="s">
+      <c r="B105" s="12" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="B105" s="14" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="B106" s="14" t="s">
+      <c r="B107" s="14" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="15" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="B107" s="16" t="s">
+      <c r="B108" s="16" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="11" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="B108" s="12" t="s">
+      <c r="B109" s="12" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="B109" s="14" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="B110" s="14" t="s">
+      <c r="B111" s="14" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="15" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="B111" s="16" t="s">
+      <c r="B112" s="16" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="B112" s="14" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="B115" s="14" t="s">
+      <c r="B116" s="14" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="11" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="B116" s="12" t="s">
+      <c r="B117" s="12" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="B117" s="14" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="B118" s="14" t="s">
+      <c r="B119" s="14" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="15" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="B119" s="16" t="s">
+      <c r="B120" s="16" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="11" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B120" s="12" t="s">
+      <c r="B121" s="12" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="B121" s="14" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B123" s="14" t="s">
+      <c r="B124" s="14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="11" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B124" s="12" t="s">
+      <c r="B125" s="12" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="B125" s="14" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="B126" s="14" t="s">
+      <c r="B127" s="14" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="15" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B127" s="16" t="s">
+      <c r="B128" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="11" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="B128" s="12" t="s">
+      <c r="B129" s="12" t="s">
         <v>262</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="B129" s="14" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="B131" s="14" t="s">
+      <c r="B132" s="14" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="11" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="B132" s="12" t="s">
+      <c r="B133" s="12" t="s">
         <v>266</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="B133" s="14" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="B134" s="14" t="s">
+      <c r="B135" s="14" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="15" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="B135" s="16" t="s">
+      <c r="B136" s="16" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="B136" s="14" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="B139" s="14" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="B139" s="14" t="s">
+      <c r="B140" s="14" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="11" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="B140" s="12" t="s">
+      <c r="B141" s="12" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="B141" s="14" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B142" s="14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="B142" s="14" t="s">
+      <c r="B143" s="14" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" s="15" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="15" t="s">
         <v>297</v>
       </c>
-      <c r="B143" s="16" t="s">
+      <c r="B144" s="16" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="11" t="s">
+    <row r="145" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A145" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="B144" s="12" t="s">
+      <c r="B145" s="12" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="145" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A145" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="B145" s="14" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="146" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A146" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="B146" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="147" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A147" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="B146" s="14" t="s">
+      <c r="B147" s="14" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="147" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A147" s="15" t="s">
+    <row r="148" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A148" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="B147" s="16" t="s">
+      <c r="B148" s="16" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="148" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A148" s="11" t="s">
+    <row r="149" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A149" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B148" s="12" t="s">
+      <c r="B149" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="R148" s="9"/>
-      <c r="S148" s="9"/>
-      <c r="T148" s="9"/>
-      <c r="U148" s="9"/>
-      <c r="V148" s="9"/>
-      <c r="W148" s="9"/>
-      <c r="X148" s="9"/>
-      <c r="Y148" s="9"/>
-      <c r="Z148" s="9"/>
-      <c r="AA148" s="9"/>
-    </row>
-    <row r="149" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A149" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B149" s="14" t="s">
-        <v>112</v>
       </c>
       <c r="R149" s="9"/>
       <c r="S149" s="9"/>
@@ -2748,10 +2774,10 @@
     </row>
     <row r="150" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A150" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B150" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R150" s="9"/>
       <c r="S150" s="9"/>
@@ -2766,10 +2792,10 @@
     </row>
     <row r="151" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A151" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B151" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R151" s="9"/>
       <c r="S151" s="9"/>
@@ -2783,66 +2809,65 @@
       <c r="AA151" s="9"/>
     </row>
     <row r="152" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A152" s="11" t="s">
+      <c r="A152" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B152" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="R152" s="9"/>
+      <c r="S152" s="9"/>
+      <c r="T152" s="9"/>
+      <c r="U152" s="9"/>
+      <c r="V152" s="9"/>
+      <c r="W152" s="9"/>
+      <c r="X152" s="9"/>
+      <c r="Y152" s="9"/>
+      <c r="Z152" s="9"/>
+      <c r="AA152" s="9"/>
+    </row>
+    <row r="153" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A153" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B152" s="12" t="s">
+      <c r="B153" s="12" t="s">
         <v>172</v>
-      </c>
-      <c r="C152"/>
-    </row>
-    <row r="153" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A153" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="B153" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="C153"/>
     </row>
     <row r="154" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A154" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B154" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C154"/>
+    </row>
+    <row r="155" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A155" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B154" s="14" t="s">
+      <c r="B155" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="C154"/>
-    </row>
-    <row r="155" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A155" s="15" t="s">
+      <c r="C155"/>
+    </row>
+    <row r="156" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A156" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B155" s="14" t="s">
+      <c r="B156" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="C155"/>
-    </row>
-    <row r="156" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A156" s="11" t="s">
+      <c r="C156"/>
+    </row>
+    <row r="157" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A157" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B156" s="12" t="s">
+      <c r="B157" s="12" t="s">
         <v>176</v>
-      </c>
-      <c r="C156"/>
-      <c r="Q156" s="9"/>
-      <c r="R156" s="9"/>
-      <c r="S156" s="9"/>
-      <c r="T156" s="9"/>
-      <c r="U156" s="9"/>
-      <c r="V156" s="9"/>
-      <c r="W156" s="9"/>
-      <c r="X156" s="9"/>
-      <c r="Y156" s="9"/>
-      <c r="Z156" s="9"/>
-    </row>
-    <row r="157" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A157" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B157" s="14" t="s">
-        <v>177</v>
       </c>
       <c r="C157"/>
       <c r="Q157" s="9"/>
@@ -2858,10 +2883,10 @@
     </row>
     <row r="158" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A158" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B158" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C158"/>
       <c r="Q158" s="9"/>
@@ -2877,10 +2902,10 @@
     </row>
     <row r="159" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A159" s="13" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C159"/>
       <c r="Q159" s="9"/>
@@ -2896,10 +2921,10 @@
     </row>
     <row r="160" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A160" s="13" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C160"/>
       <c r="Q160" s="9"/>
@@ -2915,10 +2940,10 @@
     </row>
     <row r="161" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A161" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B161" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C161"/>
       <c r="Q161" s="9"/>
@@ -2934,401 +2959,462 @@
     </row>
     <row r="162" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A162" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B162" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C162"/>
+      <c r="Q162" s="9"/>
+      <c r="R162" s="9"/>
+      <c r="S162" s="9"/>
+      <c r="T162" s="9"/>
+      <c r="U162" s="9"/>
+      <c r="V162" s="9"/>
+      <c r="W162" s="9"/>
+      <c r="X162" s="9"/>
+      <c r="Y162" s="9"/>
+      <c r="Z162" s="9"/>
+    </row>
+    <row r="163" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A163" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B162" s="14" t="s">
+      <c r="B163" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="C162"/>
-      <c r="O162" s="22"/>
-    </row>
-    <row r="163" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A163" s="15" t="s">
+      <c r="C163"/>
+      <c r="O163" s="22"/>
+    </row>
+    <row r="164" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A164" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B163" s="14" t="s">
+      <c r="B164" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="C163"/>
-    </row>
-    <row r="164" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A164" s="11" t="s">
+      <c r="C164"/>
+    </row>
+    <row r="165" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A165" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B164" s="19" t="s">
+      <c r="B165" s="19" t="s">
         <v>184</v>
-      </c>
-      <c r="C164"/>
-    </row>
-    <row r="165" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A165" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B165" s="20" t="s">
-        <v>185</v>
       </c>
       <c r="C165"/>
     </row>
     <row r="166" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A166" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B166" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C166"/>
     </row>
     <row r="167" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A167" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B167" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C167"/>
     </row>
     <row r="168" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A168" s="13" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B168" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C168"/>
     </row>
     <row r="169" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A169" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B169" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C169"/>
     </row>
     <row r="170" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A170" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B170" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="C170"/>
+    </row>
+    <row r="171" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A171" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B170" s="20" t="s">
+      <c r="B171" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="C170"/>
-    </row>
-    <row r="171" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A171" s="15" t="s">
+      <c r="C171"/>
+    </row>
+    <row r="172" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A172" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B171" s="20" t="s">
+      <c r="B172" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="C171"/>
-    </row>
-    <row r="172" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A172" s="11" t="s">
+      <c r="C172"/>
+    </row>
+    <row r="173" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A173" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B172" s="19" t="s">
+      <c r="B173" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="C172"/>
-    </row>
-    <row r="173" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A173" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B173" s="20" t="s">
-        <v>138</v>
       </c>
       <c r="C173"/>
     </row>
     <row r="174" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A174" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B174" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C174"/>
     </row>
     <row r="175" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A175" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B175" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C175"/>
     </row>
     <row r="176" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A176" s="13" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B176" s="20" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="C176"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B177" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C177"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B178" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C178"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B178" s="20" t="s">
+      <c r="B179" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="C178"/>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179" s="15" t="s">
+      <c r="C179"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="B179" s="21" t="s">
+      <c r="B180" s="21" t="s">
         <v>134</v>
-      </c>
-      <c r="C179"/>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A180" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B180" s="12" t="s">
-        <v>192</v>
       </c>
       <c r="C180"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B181" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C181"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B182" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C182"/>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="B182" s="12" t="s">
+      <c r="B183" s="12" t="s">
         <v>194</v>
-      </c>
-      <c r="C182"/>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A183" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="B183" s="18" t="s">
-        <v>195</v>
       </c>
       <c r="C183"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="17" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="B184" s="18" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="C184"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B185" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C185"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B185" s="18" t="s">
+      <c r="B186" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="C185"/>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A186" s="11" t="s">
+      <c r="C186"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B186" s="12" t="s">
+      <c r="B187" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="C186"/>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A187" s="15" t="s">
+      <c r="C187"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B187" s="21" t="s">
+      <c r="B188" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="C187"/>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A188" s="11" t="s">
+      <c r="C188"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B188" s="19" t="s">
+      <c r="B189" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="C188"/>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A189" s="15" t="s">
+      <c r="C189"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="B189" s="21" t="s">
+      <c r="B190" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="C189"/>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A190" s="17" t="s">
+      <c r="C190"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="B190" s="23" t="s">
+      <c r="B191" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="C190"/>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A191" s="24" t="s">
+      <c r="C191"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="B191" s="12" t="s">
+      <c r="B192" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C191"/>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A192" s="7" t="s">
+      <c r="C192"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B192" s="16" t="s">
+      <c r="B193" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C192"/>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193" s="5" t="s">
+      <c r="C193"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B193" s="19" t="s">
+      <c r="B194" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="C193"/>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194" s="8" t="s">
+      <c r="C194"/>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B194" s="23" t="s">
+      <c r="B195" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="C194"/>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195" s="6" t="s">
+      <c r="C195"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B195" s="20" t="s">
+      <c r="B196" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="C195"/>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196" s="7" t="s">
+      <c r="C196"/>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B196" s="21" t="s">
+      <c r="B197" s="21" t="s">
         <v>200</v>
-      </c>
-      <c r="C196"/>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B197" s="20" t="s">
-        <v>202</v>
       </c>
       <c r="C197"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B198" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C198"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B199" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C199"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B199" s="20" t="s">
+      <c r="B200" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="C199"/>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200" s="7" t="s">
+      <c r="C200"/>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B200" s="21" t="s">
+      <c r="B201" s="21" t="s">
         <v>205</v>
-      </c>
-      <c r="C200"/>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A201" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="B201" s="14" t="s">
-        <v>306</v>
       </c>
       <c r="C201"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B202" s="14" t="s">
-        <v>307</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="C202"/>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B203" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B204" s="14" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A205" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="B204" s="14" t="s">
+      <c r="B205" s="14" t="s">
         <v>309</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A206" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
         <v>353</v>
       </c>
     </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>354</v>
+      </c>
+      <c r="B209" s="10" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>358</v>
+      </c>
+      <c r="B212" s="10" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>360</v>
+      </c>
+      <c r="B213" s="10" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>364</v>
+      </c>
+      <c r="B214" s="10" t="s">
+        <v>365</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="Q162:Z162">
+  <conditionalFormatting sqref="Q163:Z163">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
added dis features to v3
</commit_message>
<xml_diff>
--- a/output/features/feature_ideas_v2.xlsx
+++ b/output/features/feature_ideas_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward Sims\Documents\ml_projects\nerdycat\nfl-big-data-bowl\output\features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6DDD29-C1EA-4251-9F4C-F90913B82456}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B8C14D-884D-4B50-861E-FBFF2A91FCF0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A745776-B911-4206-8911-3B0816B3A891}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="485">
   <si>
     <t>PlayId</t>
   </si>
@@ -630,9 +630,6 @@
     <t>Angle between rusher direction and nearest defense direction</t>
   </si>
   <si>
-    <t xml:space="preserve">how many looking at rb? </t>
-  </si>
-  <si>
     <t>Avg angle between rusher location and defense direction</t>
   </si>
   <si>
@@ -1077,9 +1074,6 @@
     <t>Number of defenders between 6 and 9 yards from line of scrimmage</t>
   </si>
   <si>
-    <t>A,S etc of general positions</t>
-  </si>
-  <si>
     <t xml:space="preserve">WR fake or block? </t>
   </si>
   <si>
@@ -1177,6 +1171,321 @@
   </si>
   <si>
     <t>NoDefenders6_8YL</t>
+  </si>
+  <si>
+    <t>force=m*a</t>
+  </si>
+  <si>
+    <t>momentum=m*v</t>
+  </si>
+  <si>
+    <t>use for 2D collision mechanics</t>
+  </si>
+  <si>
+    <t>AvgHoleSize</t>
+  </si>
+  <si>
+    <t>MinHoleSize</t>
+  </si>
+  <si>
+    <t>MaxHoleSize</t>
+  </si>
+  <si>
+    <t>StdHoleSize</t>
+  </si>
+  <si>
+    <t>AvgRusherDisHole</t>
+  </si>
+  <si>
+    <t>MaxRusherDisHole</t>
+  </si>
+  <si>
+    <t>StdRusherDisHole</t>
+  </si>
+  <si>
+    <t>MinRusherDisHole</t>
+  </si>
+  <si>
+    <t>RusherDirMinusAvgOffenseDir</t>
+  </si>
+  <si>
+    <t>AvgDefenseErrorRusherDir</t>
+  </si>
+  <si>
+    <t>MinDefenseErrorRusherDir</t>
+  </si>
+  <si>
+    <t>MaxDefenseErrorRusherDir</t>
+  </si>
+  <si>
+    <t>StdDefenseErrorRusherDir</t>
+  </si>
+  <si>
+    <t>Avg euclidean distance between rusher coordinate and defense dir function</t>
+  </si>
+  <si>
+    <t>Min euclidean distance between rusher coordinate and defense dir function</t>
+  </si>
+  <si>
+    <t>Max euclidean distance between rusher coordinate and defense dir function</t>
+  </si>
+  <si>
+    <t>Std euclidean distance between rusher coordinate and defense dir function</t>
+  </si>
+  <si>
+    <t>AvgDefenseErrorRusherOtation</t>
+  </si>
+  <si>
+    <t>Avg euclidean distance between rusher coordinate and defense Otation function</t>
+  </si>
+  <si>
+    <t>MinDefenseErrorRusherOtation</t>
+  </si>
+  <si>
+    <t>Min euclidean distance between rusher coordinate and defense Otation function</t>
+  </si>
+  <si>
+    <t>MaxDefenseErrorRusherOtation</t>
+  </si>
+  <si>
+    <t>Max euclidean distance between rusher coordinate and defense Otation function</t>
+  </si>
+  <si>
+    <t>StdDefenseErrorRusherOtation</t>
+  </si>
+  <si>
+    <t>Std euclidean distance between rusher coordinate and defense Otation function</t>
+  </si>
+  <si>
+    <t>AvgOLineA</t>
+  </si>
+  <si>
+    <t>AvgDLineA</t>
+  </si>
+  <si>
+    <t>AvgLBA</t>
+  </si>
+  <si>
+    <t>MinOLineA</t>
+  </si>
+  <si>
+    <t>MaxOLineA</t>
+  </si>
+  <si>
+    <t>StdOLineA</t>
+  </si>
+  <si>
+    <t>MinDLineA</t>
+  </si>
+  <si>
+    <t>MaxDLineA</t>
+  </si>
+  <si>
+    <t>MinLBA</t>
+  </si>
+  <si>
+    <t>MaxLBA</t>
+  </si>
+  <si>
+    <t>StdLBA</t>
+  </si>
+  <si>
+    <t>AvgOLineS</t>
+  </si>
+  <si>
+    <t>MinOLineS</t>
+  </si>
+  <si>
+    <t>MaxOLineS</t>
+  </si>
+  <si>
+    <t>StdOLineS</t>
+  </si>
+  <si>
+    <t>AvgDLineS</t>
+  </si>
+  <si>
+    <t>MinDLineS</t>
+  </si>
+  <si>
+    <t>MaxDLineS</t>
+  </si>
+  <si>
+    <t>AvgLBS</t>
+  </si>
+  <si>
+    <t>MinLBS</t>
+  </si>
+  <si>
+    <t>MaxLBS</t>
+  </si>
+  <si>
+    <t>StdLBS</t>
+  </si>
+  <si>
+    <t>AvgOLineDir</t>
+  </si>
+  <si>
+    <t>MinOLineDir</t>
+  </si>
+  <si>
+    <t>MaxOLineDir</t>
+  </si>
+  <si>
+    <t>StdOLineDir</t>
+  </si>
+  <si>
+    <t>AvgDLineDir</t>
+  </si>
+  <si>
+    <t>MinDLineDir</t>
+  </si>
+  <si>
+    <t>MaxDLineDir</t>
+  </si>
+  <si>
+    <t>AvgLBDir</t>
+  </si>
+  <si>
+    <t>MinLBDir</t>
+  </si>
+  <si>
+    <t>MaxLBDir</t>
+  </si>
+  <si>
+    <t>StdLBDir</t>
+  </si>
+  <si>
+    <t>AvgOLineOtation</t>
+  </si>
+  <si>
+    <t>MinOLineOtation</t>
+  </si>
+  <si>
+    <t>MaxOLineOtation</t>
+  </si>
+  <si>
+    <t>StdOLineOtation</t>
+  </si>
+  <si>
+    <t>AvgDLineOtation</t>
+  </si>
+  <si>
+    <t>MinDLineOtation</t>
+  </si>
+  <si>
+    <t>MaxDLineOtation</t>
+  </si>
+  <si>
+    <t>AvgLBOtation</t>
+  </si>
+  <si>
+    <t>MinLBOtation</t>
+  </si>
+  <si>
+    <t>MaxLBOtation</t>
+  </si>
+  <si>
+    <t>StdLBOtation</t>
+  </si>
+  <si>
+    <t>AvgOLineDis</t>
+  </si>
+  <si>
+    <t>MinOLineDis</t>
+  </si>
+  <si>
+    <t>MaxOLineDis</t>
+  </si>
+  <si>
+    <t>StdOLineDis</t>
+  </si>
+  <si>
+    <t>AvgDLineDis</t>
+  </si>
+  <si>
+    <t>MinDLineDis</t>
+  </si>
+  <si>
+    <t>MaxDLineDis</t>
+  </si>
+  <si>
+    <t>AvgLBDis</t>
+  </si>
+  <si>
+    <t>MinLBDis</t>
+  </si>
+  <si>
+    <t>MaxLBDis</t>
+  </si>
+  <si>
+    <t>StdLBDis</t>
+  </si>
+  <si>
+    <t>AvgOLineWeight</t>
+  </si>
+  <si>
+    <t>MinOLineWeight</t>
+  </si>
+  <si>
+    <t>MaxOLineWeight</t>
+  </si>
+  <si>
+    <t>StdOLineWeight</t>
+  </si>
+  <si>
+    <t>AvgDLineWeight</t>
+  </si>
+  <si>
+    <t>MinDLineWeight</t>
+  </si>
+  <si>
+    <t>MaxDLineWeight</t>
+  </si>
+  <si>
+    <t>AvgLBWeight</t>
+  </si>
+  <si>
+    <t>MinLBWeight</t>
+  </si>
+  <si>
+    <t>MaxLBWeight</t>
+  </si>
+  <si>
+    <t>StdLBWeight</t>
+  </si>
+  <si>
+    <t>AvgOLineHeight</t>
+  </si>
+  <si>
+    <t>MinOLineHeight</t>
+  </si>
+  <si>
+    <t>MaxOLineHeight</t>
+  </si>
+  <si>
+    <t>StdOLineHeight</t>
+  </si>
+  <si>
+    <t>AvgDLineHeight</t>
+  </si>
+  <si>
+    <t>MinDLineHeight</t>
+  </si>
+  <si>
+    <t>MaxDLineHeight</t>
+  </si>
+  <si>
+    <t>AvgLBHeight</t>
+  </si>
+  <si>
+    <t>MinLBHeight</t>
+  </si>
+  <si>
+    <t>MaxLBHeight</t>
+  </si>
+  <si>
+    <t>StdLBHeight</t>
   </si>
 </sst>
 </file>
@@ -1319,13 +1628,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1335,8 +1643,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1369,6 +1675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1683,21 +1990,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19A3A37-5DA0-43E0-B55F-7B9F3DDB721C}">
-  <dimension ref="A1:AA224"/>
+  <dimension ref="A1:Y327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B193" sqref="B193"/>
+    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A308" sqref="A308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.77734375" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="69.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="9" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="5" max="5" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.33203125" customWidth="1"/>
-    <col min="14" max="33" width="9.33203125" customWidth="1"/>
+    <col min="12" max="31" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1841,119 +2147,135 @@
       </c>
       <c r="C16"/>
     </row>
-    <row r="17" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C17"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C18"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C19"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C20"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C21"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C22"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C23"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C24"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C25"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C26"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C27"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C28"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C29"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C30"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C31"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B32" s="1"/>
+      <c r="C32"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -2077,1512 +2399,2130 @@
       <c r="B48"/>
       <c r="C48"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49"/>
       <c r="C49"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B50"/>
       <c r="C50"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A51" s="20" t="s">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A51" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A52" s="22" t="s">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="23" t="s">
+      <c r="B52" s="20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A53" s="19" t="s">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A53" s="16" t="s">
+        <v>339</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A54" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A55" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A56" s="26" t="s">
         <v>340</v>
       </c>
-      <c r="B53" s="24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A54" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="B54" s="26" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A55" s="25" t="s">
-        <v>357</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A56" s="29" t="s">
+      <c r="B56" s="27" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A57" s="24" t="s">
         <v>341</v>
       </c>
-      <c r="B56" s="30" t="s">
+      <c r="B57" s="25" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A57" s="27" t="s">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A58" s="24" t="s">
         <v>342</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B58" s="25" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A58" s="27" t="s">
-        <v>343</v>
-      </c>
-      <c r="B58" s="28" t="s">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A59" s="24" t="s">
+        <v>379</v>
+      </c>
+      <c r="B59" s="25" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A59" s="27" t="s">
-        <v>381</v>
-      </c>
-      <c r="B59" s="28" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A60" s="27" t="s">
-        <v>380</v>
-      </c>
-      <c r="B60" s="28" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A61" s="29" t="s">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A60" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A61" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B61" s="30" t="s">
+      <c r="B61" s="27" t="s">
         <v>174</v>
       </c>
       <c r="C61"/>
-      <c r="Q61" s="9"/>
-      <c r="R61" s="9"/>
-      <c r="S61" s="9"/>
-      <c r="T61" s="9"/>
-      <c r="U61" s="9"/>
-      <c r="V61" s="9"/>
-      <c r="W61" s="9"/>
-      <c r="X61" s="9"/>
-      <c r="Y61" s="9"/>
-      <c r="Z61" s="9"/>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A62" s="27" t="s">
+      <c r="O61" s="8"/>
+      <c r="P61" s="8"/>
+      <c r="Q61" s="8"/>
+      <c r="R61" s="8"/>
+      <c r="S61" s="8"/>
+      <c r="T61" s="8"/>
+      <c r="U61" s="8"/>
+      <c r="V61" s="8"/>
+      <c r="W61" s="8"/>
+      <c r="X61" s="8"/>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A62" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="25" t="s">
         <v>175</v>
       </c>
       <c r="C62"/>
-      <c r="Q62" s="9"/>
-      <c r="R62" s="9"/>
-      <c r="S62" s="9"/>
-      <c r="T62" s="9"/>
-      <c r="U62" s="9"/>
-      <c r="V62" s="9"/>
-      <c r="W62" s="9"/>
-      <c r="X62" s="9"/>
-      <c r="Y62" s="9"/>
-      <c r="Z62" s="9"/>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A63" s="27" t="s">
+      <c r="O62" s="8"/>
+      <c r="P62" s="8"/>
+      <c r="Q62" s="8"/>
+      <c r="R62" s="8"/>
+      <c r="S62" s="8"/>
+      <c r="T62" s="8"/>
+      <c r="U62" s="8"/>
+      <c r="V62" s="8"/>
+      <c r="W62" s="8"/>
+      <c r="X62" s="8"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A63" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B63" s="28" t="s">
+      <c r="B63" s="25" t="s">
         <v>176</v>
       </c>
       <c r="C63"/>
-      <c r="Q63" s="9"/>
-      <c r="R63" s="9"/>
-      <c r="S63" s="9"/>
-      <c r="T63" s="9"/>
-      <c r="U63" s="9"/>
-      <c r="V63" s="9"/>
-      <c r="W63" s="9"/>
-      <c r="X63" s="9"/>
-      <c r="Y63" s="9"/>
-      <c r="Z63" s="9"/>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A64" s="27" t="s">
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="8"/>
+      <c r="R63" s="8"/>
+      <c r="S63" s="8"/>
+      <c r="T63" s="8"/>
+      <c r="U63" s="8"/>
+      <c r="V63" s="8"/>
+      <c r="W63" s="8"/>
+      <c r="X63" s="8"/>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A64" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="B64" s="28" t="s">
+      <c r="B64" s="25" t="s">
         <v>177</v>
       </c>
       <c r="C64"/>
-      <c r="Q64" s="9"/>
-      <c r="R64" s="9"/>
-      <c r="S64" s="9"/>
-      <c r="T64" s="9"/>
-      <c r="U64" s="9"/>
-      <c r="V64" s="9"/>
-      <c r="W64" s="9"/>
-      <c r="X64" s="9"/>
-      <c r="Y64" s="9"/>
-      <c r="Z64" s="9"/>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A65" s="27" t="s">
+      <c r="O64" s="8"/>
+      <c r="P64" s="8"/>
+      <c r="Q64" s="8"/>
+      <c r="R64" s="8"/>
+      <c r="S64" s="8"/>
+      <c r="T64" s="8"/>
+      <c r="U64" s="8"/>
+      <c r="V64" s="8"/>
+      <c r="W64" s="8"/>
+      <c r="X64" s="8"/>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A65" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="B65" s="28" t="s">
+      <c r="B65" s="25" t="s">
         <v>178</v>
       </c>
       <c r="C65"/>
-      <c r="Q65" s="9"/>
-      <c r="R65" s="9"/>
-      <c r="S65" s="9"/>
-      <c r="T65" s="9"/>
-      <c r="U65" s="9"/>
-      <c r="V65" s="9"/>
-      <c r="W65" s="9"/>
-      <c r="X65" s="9"/>
-      <c r="Y65" s="9"/>
-      <c r="Z65" s="9"/>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A66" s="27" t="s">
+      <c r="O65" s="8"/>
+      <c r="P65" s="8"/>
+      <c r="Q65" s="8"/>
+      <c r="R65" s="8"/>
+      <c r="S65" s="8"/>
+      <c r="T65" s="8"/>
+      <c r="U65" s="8"/>
+      <c r="V65" s="8"/>
+      <c r="W65" s="8"/>
+      <c r="X65" s="8"/>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A66" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="B66" s="28" t="s">
+      <c r="B66" s="25" t="s">
         <v>179</v>
       </c>
       <c r="C66"/>
-      <c r="Q66" s="9"/>
-      <c r="R66" s="9"/>
-      <c r="S66" s="9"/>
-      <c r="T66" s="9"/>
-      <c r="U66" s="9"/>
-      <c r="V66" s="9"/>
-      <c r="W66" s="9"/>
-      <c r="X66" s="9"/>
-      <c r="Y66" s="9"/>
-      <c r="Z66" s="9"/>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A67" s="27" t="s">
+      <c r="O66" s="8"/>
+      <c r="P66" s="8"/>
+      <c r="Q66" s="8"/>
+      <c r="R66" s="8"/>
+      <c r="S66" s="8"/>
+      <c r="T66" s="8"/>
+      <c r="U66" s="8"/>
+      <c r="V66" s="8"/>
+      <c r="W66" s="8"/>
+      <c r="X66" s="8"/>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A67" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="25" t="s">
         <v>180</v>
       </c>
       <c r="C67"/>
-      <c r="O67" s="17"/>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A68" s="32" t="s">
+      <c r="M67" s="14"/>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A68" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="B68" s="28" t="s">
+      <c r="B68" s="25" t="s">
         <v>181</v>
       </c>
       <c r="C68"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A69" s="29" t="s">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A69" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="B69" s="27"/>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A70" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="B69" s="30"/>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A70" s="27" t="s">
+      <c r="B70" s="25"/>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A71" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="B70" s="28"/>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A71" s="27" t="s">
+      <c r="B71" s="25"/>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A72" s="29" t="s">
         <v>318</v>
       </c>
-      <c r="B71" s="28"/>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A72" s="32" t="s">
+      <c r="B72" s="30"/>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B72" s="33"/>
-    </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+      <c r="B73" s="25"/>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B73" s="28"/>
-    </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+      <c r="B74" s="25"/>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B74" s="28"/>
-    </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+      <c r="B75" s="25"/>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B75" s="28"/>
-    </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+      <c r="B76" s="25"/>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A77" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="B76" s="28"/>
-    </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A77" s="29" t="s">
+      <c r="B77" s="27"/>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A78" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="B77" s="30"/>
-    </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A78" s="27" t="s">
+      <c r="B78" s="25"/>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A79" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="B78" s="28"/>
-    </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A79" s="27" t="s">
+      <c r="B79" s="25"/>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A80" s="29" t="s">
         <v>326</v>
       </c>
-      <c r="B79" s="28"/>
-    </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A80" s="32" t="s">
-        <v>327</v>
-      </c>
-      <c r="B80" s="33"/>
+      <c r="B80" s="30"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="B81" s="28"/>
+        <v>327</v>
+      </c>
+      <c r="B81" s="25"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B82" s="28"/>
+        <v>328</v>
+      </c>
+      <c r="B82" s="25"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B83" s="28"/>
+        <v>329</v>
+      </c>
+      <c r="B83" s="25"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B84" s="25"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="24" t="s">
+        <v>359</v>
+      </c>
+      <c r="B85" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="C85"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="B86" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="C86"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B87" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="C87"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="C88"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="B89" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="C89"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="B90" s="27" t="s">
+        <v>366</v>
+      </c>
+      <c r="C90"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B91" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="C91"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B92" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C92"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B93" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="C93"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B94" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="C94"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B95" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C95"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B96" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="C96"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B97" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="C97"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B98" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C98"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B99" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="C99"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B100" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="C100"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="B101" s="27"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="24" t="s">
+        <v>308</v>
+      </c>
+      <c r="B102" s="25"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="B103" s="25"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="B104" s="30"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="B105" s="25"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="B106" s="25"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="B107" s="25"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="B108" s="25"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="26" t="s">
         <v>331</v>
       </c>
-      <c r="B84" s="28"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="27" t="s">
-        <v>361</v>
-      </c>
-      <c r="B85" s="28" t="s">
-        <v>369</v>
-      </c>
-      <c r="C85"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="27" t="s">
-        <v>362</v>
-      </c>
-      <c r="B86" s="28" t="s">
-        <v>370</v>
-      </c>
-      <c r="C86"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="B87" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="C87"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="B88" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="C88"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="B89" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="C89"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="29" t="s">
-        <v>363</v>
-      </c>
-      <c r="B90" s="30" t="s">
-        <v>368</v>
-      </c>
-      <c r="C90"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="B91" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="C91"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="B92" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="C92"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="B93" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="B94" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="B95" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="B96" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="B97" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="C97"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="B98" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="C98"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="B99" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="C99"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="B100" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="C100"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="29" t="s">
-        <v>308</v>
-      </c>
-      <c r="B101" s="30"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="27" t="s">
-        <v>309</v>
-      </c>
-      <c r="B102" s="28"/>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="27" t="s">
-        <v>310</v>
-      </c>
-      <c r="B103" s="28"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="32" t="s">
-        <v>311</v>
-      </c>
-      <c r="B104" s="33"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="27" t="s">
-        <v>312</v>
-      </c>
-      <c r="B105" s="28"/>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="27" t="s">
-        <v>313</v>
-      </c>
-      <c r="B106" s="28"/>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="27" t="s">
-        <v>314</v>
-      </c>
-      <c r="B107" s="28"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="B108" s="28"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="29" t="s">
+      <c r="B109" s="27"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="24" t="s">
         <v>332</v>
       </c>
-      <c r="B109" s="30"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="27" t="s">
+      <c r="B110" s="25"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="24" t="s">
         <v>333</v>
       </c>
-      <c r="B110" s="28"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="27" t="s">
+      <c r="B111" s="25"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="29" t="s">
         <v>334</v>
       </c>
-      <c r="B111" s="28"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="32" t="s">
-        <v>335</v>
-      </c>
-      <c r="B112" s="33"/>
+      <c r="B112" s="30"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="B113" s="28"/>
+        <v>335</v>
+      </c>
+      <c r="B113" s="25"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="B114" s="28"/>
+        <v>336</v>
+      </c>
+      <c r="B114" s="25"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B115" s="28"/>
+        <v>337</v>
+      </c>
+      <c r="B115" s="25"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="B116" s="28"/>
+        <v>338</v>
+      </c>
+      <c r="B116" s="25"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="29" t="s">
+      <c r="A117" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="B117" s="30" t="s">
+      <c r="B117" s="27" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="27" t="s">
+      <c r="A118" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="B118" s="25" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="B118" s="28" t="s">
+      <c r="B119" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="27" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B120" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B121" s="27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="B119" s="28" t="s">
+      <c r="B122" s="25" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="B120" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="B121" s="30" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="27" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="B122" s="28" t="s">
+      <c r="B123" s="25" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="27" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B124" s="30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B125" s="27" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="B126" s="25" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="B127" s="25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="B128" s="30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B129" s="27" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="B130" s="25" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="B131" s="25" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="B132" s="30" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="B133" s="27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="B134" s="25" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="B135" s="25" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="B136" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="B137" s="25" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="B138" s="25" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="B139" s="25" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="B140" s="25" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="B141" s="27" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="B142" s="25" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="B143" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="B144" s="30" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B145" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B123" s="28" t="s">
+      <c r="B146" s="25" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B124" s="33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="B125" s="30" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="B126" s="28" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="B127" s="28" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="B128" s="33" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="29" t="s">
-        <v>224</v>
-      </c>
-      <c r="B129" s="30" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="27" t="s">
-        <v>225</v>
-      </c>
-      <c r="B130" s="28" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="B131" s="28" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="B132" s="33" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="29" t="s">
-        <v>236</v>
-      </c>
-      <c r="B133" s="30" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="B134" s="28" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="B135" s="28" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="32" t="s">
-        <v>239</v>
-      </c>
-      <c r="B136" s="33" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="B147" s="25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B148" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B149" s="27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="B150" s="25" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="B151" s="25" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B152" s="30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="B153" s="27" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="27" t="s">
-        <v>240</v>
-      </c>
-      <c r="B137" s="28" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="B138" s="28" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="27" t="s">
-        <v>242</v>
-      </c>
-      <c r="B139" s="28" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="B140" s="28" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="B141" s="30" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="B142" s="28" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="B143" s="28" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="32" t="s">
-        <v>247</v>
-      </c>
-      <c r="B144" s="33" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B145" s="30" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="B146" s="28" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="27" t="s">
-        <v>209</v>
-      </c>
-      <c r="B147" s="28" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="B148" s="28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B149" s="30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="27" t="s">
-        <v>210</v>
-      </c>
-      <c r="B150" s="28" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" s="27" t="s">
-        <v>211</v>
-      </c>
-      <c r="B151" s="28" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="B152" s="33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" s="29" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="B153" s="30" t="s">
+      <c r="B154" s="25" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="27" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="B154" s="28" t="s">
+      <c r="B155" s="25" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" s="27" t="s">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="B155" s="28" t="s">
+      <c r="B156" s="25" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" s="27" t="s">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" s="26" t="s">
         <v>283</v>
       </c>
-      <c r="B156" s="28" t="s">
+      <c r="B157" s="27" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" s="29" t="s">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" s="24" t="s">
         <v>284</v>
       </c>
-      <c r="B157" s="30" t="s">
+      <c r="B158" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="27" t="s">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" s="24" t="s">
         <v>285</v>
       </c>
-      <c r="B158" s="28" t="s">
+      <c r="B159" s="25" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" s="27" t="s">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="B159" s="28" t="s">
+      <c r="B160" s="30" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" s="32" t="s">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A161" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="B160" s="33" t="s">
+      <c r="B161" s="25" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="161" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A161" s="27" t="s">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A162" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="B161" s="28" t="s">
+      <c r="B162" s="25" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="162" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A162" s="27" t="s">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A163" s="24" t="s">
         <v>289</v>
       </c>
-      <c r="B162" s="28" t="s">
+      <c r="B163" s="25" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="163" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A163" s="27" t="s">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A164" s="24" t="s">
         <v>290</v>
       </c>
-      <c r="B163" s="28" t="s">
+      <c r="B164" s="25" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="164" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A164" s="27" t="s">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A165" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="B164" s="28" t="s">
+      <c r="B165" s="27" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="165" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A165" s="29" t="s">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A166" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="B165" s="30" t="s">
+      <c r="B166" s="25" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="166" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A166" s="27" t="s">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A167" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="B166" s="28" t="s">
+      <c r="B167" s="25" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="167" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A167" s="27" t="s">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A168" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="B167" s="28" t="s">
+      <c r="B168" s="30" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="168" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A168" s="32" t="s">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A169" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="B168" s="33" t="s">
+      <c r="B169" s="27" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="169" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A169" s="29" t="s">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A170" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="B169" s="30" t="s">
+      <c r="B170" s="25" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="170" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A170" s="27" t="s">
+    <row r="171" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A171" s="24" t="s">
         <v>297</v>
       </c>
-      <c r="B170" s="28" t="s">
+      <c r="B171" s="25" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="171" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A171" s="27" t="s">
+    <row r="172" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A172" s="29" t="s">
         <v>298</v>
       </c>
-      <c r="B171" s="28" t="s">
+      <c r="B172" s="30" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="172" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A172" s="32" t="s">
+    <row r="173" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A173" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B173" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="P173" s="8"/>
+      <c r="Q173" s="8"/>
+      <c r="R173" s="8"/>
+      <c r="S173" s="8"/>
+      <c r="T173" s="8"/>
+      <c r="U173" s="8"/>
+      <c r="V173" s="8"/>
+      <c r="W173" s="8"/>
+      <c r="X173" s="8"/>
+      <c r="Y173" s="8"/>
+    </row>
+    <row r="174" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A174" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="B174" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="P174" s="8"/>
+      <c r="Q174" s="8"/>
+      <c r="R174" s="8"/>
+      <c r="S174" s="8"/>
+      <c r="T174" s="8"/>
+      <c r="U174" s="8"/>
+      <c r="V174" s="8"/>
+      <c r="W174" s="8"/>
+      <c r="X174" s="8"/>
+      <c r="Y174" s="8"/>
+    </row>
+    <row r="175" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A175" s="24" t="s">
+        <v>372</v>
+      </c>
+      <c r="B175" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="P175" s="8"/>
+      <c r="Q175" s="8"/>
+      <c r="R175" s="8"/>
+      <c r="S175" s="8"/>
+      <c r="T175" s="8"/>
+      <c r="U175" s="8"/>
+      <c r="V175" s="8"/>
+      <c r="W175" s="8"/>
+      <c r="X175" s="8"/>
+      <c r="Y175" s="8"/>
+    </row>
+    <row r="176" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A176" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B176" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="P176" s="8"/>
+      <c r="Q176" s="8"/>
+      <c r="R176" s="8"/>
+      <c r="S176" s="8"/>
+      <c r="T176" s="8"/>
+      <c r="U176" s="8"/>
+      <c r="V176" s="8"/>
+      <c r="W176" s="8"/>
+      <c r="X176" s="8"/>
+      <c r="Y176" s="8"/>
+    </row>
+    <row r="177" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A177" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B177" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="P177" s="8"/>
+      <c r="Q177" s="8"/>
+      <c r="R177" s="8"/>
+      <c r="S177" s="8"/>
+      <c r="T177" s="8"/>
+      <c r="U177" s="8"/>
+      <c r="V177" s="8"/>
+      <c r="W177" s="8"/>
+      <c r="X177" s="8"/>
+      <c r="Y177" s="8"/>
+    </row>
+    <row r="178" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A178" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="B178" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="P178" s="8"/>
+      <c r="Q178" s="8"/>
+      <c r="R178" s="8"/>
+      <c r="S178" s="8"/>
+      <c r="T178" s="8"/>
+      <c r="U178" s="8"/>
+      <c r="V178" s="8"/>
+      <c r="W178" s="8"/>
+      <c r="X178" s="8"/>
+      <c r="Y178" s="8"/>
+    </row>
+    <row r="179" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A179" s="24" t="s">
+        <v>370</v>
+      </c>
+      <c r="B179" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="P179" s="8"/>
+      <c r="Q179" s="8"/>
+      <c r="R179" s="8"/>
+      <c r="S179" s="8"/>
+      <c r="T179" s="8"/>
+      <c r="U179" s="8"/>
+      <c r="V179" s="8"/>
+      <c r="W179" s="8"/>
+      <c r="X179" s="8"/>
+      <c r="Y179" s="8"/>
+    </row>
+    <row r="180" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A180" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B180" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="P180" s="8"/>
+      <c r="Q180" s="8"/>
+      <c r="R180" s="8"/>
+      <c r="S180" s="8"/>
+      <c r="T180" s="8"/>
+      <c r="U180" s="8"/>
+      <c r="V180" s="8"/>
+      <c r="W180" s="8"/>
+      <c r="X180" s="8"/>
+      <c r="Y180" s="8"/>
+    </row>
+    <row r="181" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A181" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B181" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="C181"/>
+    </row>
+    <row r="182" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A182" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B182" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="C182"/>
+    </row>
+    <row r="183" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A183" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B183" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C183"/>
+    </row>
+    <row r="184" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A184" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B184" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C184"/>
+    </row>
+    <row r="185" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A185" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="B185" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C185"/>
+    </row>
+    <row r="186" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A186" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B186" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C186"/>
+    </row>
+    <row r="187" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A187" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B187" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C187"/>
+    </row>
+    <row r="188" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A188" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B188" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C188"/>
+    </row>
+    <row r="189" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A189" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B189" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C189"/>
+    </row>
+    <row r="190" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A190" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B190" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C190"/>
+    </row>
+    <row r="191" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A191" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B191" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C191"/>
+    </row>
+    <row r="192" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A192" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B192" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C192"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B193" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C193"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B194" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="C194"/>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B195" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="C195"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B196" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C196"/>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B197" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C197"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B198" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C198"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B199" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C199"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="B200" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="C200"/>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B201" s="34"/>
+      <c r="C201"/>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B202" s="34"/>
+      <c r="C202"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A203" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B203" s="34"/>
+      <c r="C203"/>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B204" s="34"/>
+      <c r="C204"/>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A205" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B205" s="34"/>
+      <c r="C205"/>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B206" s="34"/>
+      <c r="C206"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A207" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B207" s="34"/>
+      <c r="C207"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B208" s="34"/>
+      <c r="C208"/>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A209" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B209" s="34"/>
+      <c r="C209"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A210" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B210" s="34"/>
+      <c r="C210"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A211" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B211" s="34"/>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A212" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B212" s="34"/>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A213" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B213" s="34"/>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A214" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B214" s="34"/>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A215" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B215" s="34"/>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A216" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B216" s="34"/>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A217" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B217" s="34"/>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A218" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B218" s="34"/>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A219" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B219" s="34"/>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B220" s="34"/>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A221" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B221" s="34"/>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A222" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B222" s="34"/>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A223" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B223" s="34"/>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A224" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B224" s="34"/>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" s="34" t="s">
+        <v>430</v>
+      </c>
+      <c r="B225" s="34"/>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" s="34" t="s">
+        <v>431</v>
+      </c>
+      <c r="B226" s="34"/>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227" s="34" t="s">
+        <v>432</v>
+      </c>
+      <c r="B227" s="34"/>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A228" s="34" t="s">
+        <v>433</v>
+      </c>
+      <c r="B228" s="34"/>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A229" s="34" t="s">
+        <v>434</v>
+      </c>
+      <c r="B229" s="34"/>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A230" s="34" t="s">
+        <v>435</v>
+      </c>
+      <c r="B230" s="34"/>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A231" s="34" t="s">
+        <v>436</v>
+      </c>
+      <c r="B231" s="34"/>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A232" s="34" t="s">
+        <v>434</v>
+      </c>
+      <c r="B232" s="34"/>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A233" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="B233" s="34"/>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A234" s="34" t="s">
+        <v>438</v>
+      </c>
+      <c r="B234" s="34"/>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A235" s="34" t="s">
+        <v>439</v>
+      </c>
+      <c r="B235" s="34"/>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A236" s="34" t="s">
+        <v>440</v>
+      </c>
+      <c r="B236" s="34"/>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A237" s="34" t="s">
+        <v>441</v>
+      </c>
+      <c r="B237" s="34"/>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A238" s="34" t="s">
+        <v>442</v>
+      </c>
+      <c r="B238" s="34"/>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A239" s="34" t="s">
+        <v>443</v>
+      </c>
+      <c r="B239" s="34"/>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A240" s="34" t="s">
+        <v>444</v>
+      </c>
+      <c r="B240" s="34"/>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A241" s="34" t="s">
+        <v>445</v>
+      </c>
+      <c r="B241" s="34"/>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A242" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="B242" s="34"/>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A243" s="34" t="s">
+        <v>447</v>
+      </c>
+      <c r="B243" s="34"/>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A244" s="34" t="s">
+        <v>445</v>
+      </c>
+      <c r="B244" s="34"/>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A245" s="34" t="s">
+        <v>448</v>
+      </c>
+      <c r="B245" s="34"/>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A246" s="34" t="s">
+        <v>449</v>
+      </c>
+      <c r="B246" s="34"/>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A247" s="34" t="s">
+        <v>450</v>
+      </c>
+      <c r="B247" s="34"/>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A248" s="34" t="s">
+        <v>451</v>
+      </c>
+      <c r="B248" s="34"/>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A249" s="34" t="s">
+        <v>452</v>
+      </c>
+      <c r="B249" s="34"/>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A250" s="34" t="s">
+        <v>453</v>
+      </c>
+      <c r="B250" s="34"/>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A251" s="34" t="s">
+        <v>454</v>
+      </c>
+      <c r="B251" s="34"/>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A252" s="34" t="s">
+        <v>455</v>
+      </c>
+      <c r="B252" s="34"/>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A253" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="B253" s="34"/>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A254" s="34" t="s">
+        <v>457</v>
+      </c>
+      <c r="B254" s="34"/>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A255" s="34" t="s">
+        <v>458</v>
+      </c>
+      <c r="B255" s="34"/>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A256" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="B256" s="34"/>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A257" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="B257" s="34"/>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A258" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="B258" s="34"/>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A259" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="B259" s="34"/>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A260" s="34" t="s">
+        <v>462</v>
+      </c>
+      <c r="B260" s="34"/>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A261" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="B261" s="34"/>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A262" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="B262" s="34"/>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A263" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="B263" s="34"/>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A264" s="34" t="s">
+        <v>466</v>
+      </c>
+      <c r="B264" s="34"/>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265" s="34" t="s">
+        <v>467</v>
+      </c>
+      <c r="B265" s="34"/>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A266" s="34" t="s">
+        <v>468</v>
+      </c>
+      <c r="B266" s="34"/>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A267" s="34" t="s">
+        <v>469</v>
+      </c>
+      <c r="B267" s="34"/>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A268" s="34" t="s">
+        <v>467</v>
+      </c>
+      <c r="B268" s="34"/>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A269" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="B269" s="34"/>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A270" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="B270" s="34"/>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A271" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="B271" s="34"/>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A272" s="34" t="s">
+        <v>473</v>
+      </c>
+      <c r="B272" s="34"/>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A273" s="34" t="s">
+        <v>474</v>
+      </c>
+      <c r="B273" s="34"/>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A274" s="34" t="s">
+        <v>475</v>
+      </c>
+      <c r="B274" s="34"/>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A275" s="34" t="s">
+        <v>476</v>
+      </c>
+      <c r="B275" s="34"/>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A276" s="34" t="s">
+        <v>477</v>
+      </c>
+      <c r="B276" s="34"/>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A277" s="34" t="s">
+        <v>478</v>
+      </c>
+      <c r="B277" s="34"/>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A278" s="34" t="s">
+        <v>479</v>
+      </c>
+      <c r="B278" s="34"/>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A279" s="34" t="s">
+        <v>480</v>
+      </c>
+      <c r="B279" s="34"/>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A280" s="34" t="s">
+        <v>478</v>
+      </c>
+      <c r="B280" s="34"/>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A281" s="34" t="s">
+        <v>481</v>
+      </c>
+      <c r="B281" s="34"/>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A282" s="34" t="s">
+        <v>482</v>
+      </c>
+      <c r="B282" s="34"/>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A283" s="34" t="s">
+        <v>483</v>
+      </c>
+      <c r="B283" s="34"/>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A284" s="34" t="s">
+        <v>484</v>
+      </c>
+      <c r="B284" s="25" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A285" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="B285" s="11" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A286" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B286" s="15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A287" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B287" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A288" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B288" s="13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A289" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B289" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A290" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B290" s="12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A291" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B291" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A292" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B292" s="13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A293" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B293" s="11" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A294" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="B172" s="33" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="173" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A173" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="B173" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="R173" s="9"/>
-      <c r="S173" s="9"/>
-      <c r="T173" s="9"/>
-      <c r="U173" s="9"/>
-      <c r="V173" s="9"/>
-      <c r="W173" s="9"/>
-      <c r="X173" s="9"/>
-      <c r="Y173" s="9"/>
-      <c r="Z173" s="9"/>
-      <c r="AA173" s="9"/>
-    </row>
-    <row r="174" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A174" s="35" t="s">
-        <v>373</v>
-      </c>
-      <c r="B174" s="28" t="s">
-        <v>377</v>
-      </c>
-      <c r="R174" s="9"/>
-      <c r="S174" s="9"/>
-      <c r="T174" s="9"/>
-      <c r="U174" s="9"/>
-      <c r="V174" s="9"/>
-      <c r="W174" s="9"/>
-      <c r="X174" s="9"/>
-      <c r="Y174" s="9"/>
-      <c r="Z174" s="9"/>
-      <c r="AA174" s="9"/>
-    </row>
-    <row r="175" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A175" s="27" t="s">
-        <v>374</v>
-      </c>
-      <c r="B175" s="28" t="s">
-        <v>378</v>
-      </c>
-      <c r="R175" s="9"/>
-      <c r="S175" s="9"/>
-      <c r="T175" s="9"/>
-      <c r="U175" s="9"/>
-      <c r="V175" s="9"/>
-      <c r="W175" s="9"/>
-      <c r="X175" s="9"/>
-      <c r="Y175" s="9"/>
-      <c r="Z175" s="9"/>
-      <c r="AA175" s="9"/>
-    </row>
-    <row r="176" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A176" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="B176" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="R176" s="9"/>
-      <c r="S176" s="9"/>
-      <c r="T176" s="9"/>
-      <c r="U176" s="9"/>
-      <c r="V176" s="9"/>
-      <c r="W176" s="9"/>
-      <c r="X176" s="9"/>
-      <c r="Y176" s="9"/>
-      <c r="Z176" s="9"/>
-      <c r="AA176" s="9"/>
-    </row>
-    <row r="177" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A177" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="B177" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="R177" s="9"/>
-      <c r="S177" s="9"/>
-      <c r="T177" s="9"/>
-      <c r="U177" s="9"/>
-      <c r="V177" s="9"/>
-      <c r="W177" s="9"/>
-      <c r="X177" s="9"/>
-      <c r="Y177" s="9"/>
-      <c r="Z177" s="9"/>
-      <c r="AA177" s="9"/>
-    </row>
-    <row r="178" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A178" s="27" t="s">
-        <v>371</v>
-      </c>
-      <c r="B178" s="28" t="s">
-        <v>375</v>
-      </c>
-      <c r="R178" s="9"/>
-      <c r="S178" s="9"/>
-      <c r="T178" s="9"/>
-      <c r="U178" s="9"/>
-      <c r="V178" s="9"/>
-      <c r="W178" s="9"/>
-      <c r="X178" s="9"/>
-      <c r="Y178" s="9"/>
-      <c r="Z178" s="9"/>
-      <c r="AA178" s="9"/>
-    </row>
-    <row r="179" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A179" s="27" t="s">
-        <v>372</v>
-      </c>
-      <c r="B179" s="28" t="s">
-        <v>376</v>
-      </c>
-      <c r="R179" s="9"/>
-      <c r="S179" s="9"/>
-      <c r="T179" s="9"/>
-      <c r="U179" s="9"/>
-      <c r="V179" s="9"/>
-      <c r="W179" s="9"/>
-      <c r="X179" s="9"/>
-      <c r="Y179" s="9"/>
-      <c r="Z179" s="9"/>
-      <c r="AA179" s="9"/>
-    </row>
-    <row r="180" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A180" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="B180" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="R180" s="9"/>
-      <c r="S180" s="9"/>
-      <c r="T180" s="9"/>
-      <c r="U180" s="9"/>
-      <c r="V180" s="9"/>
-      <c r="W180" s="9"/>
-      <c r="X180" s="9"/>
-      <c r="Y180" s="9"/>
-      <c r="Z180" s="9"/>
-      <c r="AA180" s="9"/>
-    </row>
-    <row r="181" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A181" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="B181" s="30" t="s">
-        <v>170</v>
-      </c>
-      <c r="C181"/>
-    </row>
-    <row r="182" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A182" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="B182" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="C182"/>
-    </row>
-    <row r="183" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A183" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="B183" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="C183"/>
-    </row>
-    <row r="184" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A184" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="B184" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="C184"/>
-    </row>
-    <row r="185" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A185" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="B185" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="C185"/>
-    </row>
-    <row r="186" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A186" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="B186" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="C186"/>
-    </row>
-    <row r="187" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A187" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="B187" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="C187"/>
-    </row>
-    <row r="188" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A188" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="B188" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="C188"/>
-    </row>
-    <row r="189" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A189" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="B189" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="C189"/>
-    </row>
-    <row r="190" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A190" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B190" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="C190"/>
-    </row>
-    <row r="191" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A191" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="B191" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="C191"/>
-    </row>
-    <row r="192" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A192" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="B192" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="C192"/>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="B193" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="C193"/>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="B194" s="33" t="s">
-        <v>195</v>
-      </c>
-      <c r="C194"/>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="B195" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C195"/>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="B196" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="C196"/>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="B197" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="C197"/>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A198" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="B198" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="C198"/>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A199" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="B199" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C199"/>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="B200" s="12" t="s">
-        <v>366</v>
-      </c>
-      <c r="C200"/>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A201" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="B201" s="12" t="s">
-        <v>367</v>
-      </c>
-      <c r="C201"/>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A202" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B202" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="C202"/>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A203" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B203" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="C203"/>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A204" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B204" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="C204"/>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A205" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B205" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="C205"/>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A206" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B206" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="C206"/>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A207" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B207" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="C207"/>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A208" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B208" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="C208"/>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A209" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B209" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="C209"/>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A210" s="11" t="s">
+      <c r="B294" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A295" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="B210" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="C210"/>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A211" s="11" t="s">
+      <c r="B295" s="11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A296" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="B211" s="12" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A212" s="11" t="s">
+      <c r="B296" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A297" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="B212" s="12" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A213" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="B213" s="12" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A214" s="31"/>
-      <c r="B214" s="34"/>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A215" s="31"/>
-      <c r="B215" s="34"/>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A217" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A218" t="s">
+      <c r="B297" s="31"/>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A298" s="28"/>
+      <c r="B298" s="31"/>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A299" s="28"/>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A309" t="s">
+        <v>392</v>
+      </c>
+      <c r="B309" s="9" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
+        <v>393</v>
+      </c>
+      <c r="B310" s="9" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
+        <v>394</v>
+      </c>
+      <c r="B311" s="9" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
+        <v>395</v>
+      </c>
+      <c r="B312" s="9" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A313" t="s">
+        <v>400</v>
+      </c>
+      <c r="B313" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A314" t="s">
+        <v>402</v>
+      </c>
+      <c r="B314" s="9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>404</v>
+      </c>
+      <c r="B315" s="9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A316" t="s">
+        <v>406</v>
+      </c>
+      <c r="B316" s="9" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A317" s="9"/>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A320" t="s">
+        <v>347</v>
+      </c>
+      <c r="B320" s="9" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A219" t="s">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A321" t="s">
         <v>349</v>
       </c>
-      <c r="B219" s="10" t="s">
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A322" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A220" t="s">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A323" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A221" t="s">
+      <c r="B323" s="9" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A222" t="s">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
         <v>353</v>
       </c>
-      <c r="B222" s="10" t="s">
+      <c r="B324" s="9" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A223" t="s">
-        <v>355</v>
-      </c>
-      <c r="B223" s="10" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A224" t="s">
-        <v>359</v>
-      </c>
-      <c r="B224" s="10" t="s">
-        <v>360</v>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
+        <v>357</v>
+      </c>
+      <c r="B325" s="9" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>381</v>
+      </c>
+      <c r="B327" s="9" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Q67:Z67">
+  <conditionalFormatting sqref="O67:X67">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>